<commit_message>
IQC creator v1.0 20221228-007
</commit_message>
<xml_diff>
--- a/list_V02.xlsx
+++ b/list_V02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zz\PycharmProjects\IQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA085661-71F6-45D5-8195-25C49F62696A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA577BD1-555F-4D5B-BDA0-11AF3830DD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" tabRatio="458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BP$324</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$CH$324</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12830" uniqueCount="2357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12834" uniqueCount="2361">
   <si>
     <t>物料号</t>
   </si>
@@ -7895,6 +7895,22 @@
   </si>
   <si>
     <t>检验图纸中椭圆圈出的内容</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺寸9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺寸10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺寸11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺寸12</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8103,7 +8119,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8292,6 +8308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8540,7 +8562,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8600,6 +8622,15 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -8970,11 +9001,11 @@
   <dimension ref="A1:CH324"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="13" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="1" topLeftCell="BR2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="BJ16" sqref="BJ16"/>
+      <selection pane="bottomRight" activeCell="C175" sqref="A175:XFD175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9050,7 +9081,7 @@
     <col min="81" max="16384" width="8.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:82" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1484</v>
       </c>
@@ -9285,8 +9316,20 @@
       <c r="BZ1" s="4" t="s">
         <v>1988</v>
       </c>
+      <c r="CA1" s="4" t="s">
+        <v>2357</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>2358</v>
+      </c>
+      <c r="CC1" s="4" t="s">
+        <v>2359</v>
+      </c>
+      <c r="CD1" s="4" t="s">
+        <v>2360</v>
+      </c>
     </row>
-    <row r="2" spans="1:78" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:82" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>275</v>
       </c>
@@ -9456,7 +9499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:82" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>276</v>
       </c>
@@ -9626,7 +9669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>241</v>
       </c>
@@ -9796,7 +9839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>243</v>
       </c>
@@ -9966,7 +10009,7 @@
         <v>1551</v>
       </c>
     </row>
-    <row r="6" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>262</v>
       </c>
@@ -10118,7 +10161,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="7" spans="1:78" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:82" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
         <v>7</v>
       </c>
@@ -10285,7 +10328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:78" s="12" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:82" s="12" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>273</v>
       </c>
@@ -10455,7 +10498,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="9" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>260</v>
       </c>
@@ -10625,7 +10668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>259</v>
       </c>
@@ -10777,7 +10820,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="11" spans="1:78" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:82" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>263</v>
       </c>
@@ -10929,7 +10972,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:82" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>236</v>
       </c>
@@ -11081,7 +11124,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="13" spans="1:78" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:82" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>109</v>
       </c>
@@ -11224,7 +11267,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:78" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:82" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>110</v>
       </c>
@@ -11364,7 +11407,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:78" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:82" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>111</v>
       </c>
@@ -11510,7 +11553,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:78" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:82" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>112</v>
       </c>
@@ -16798,17 +16841,17 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="53" spans="1:79" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:79" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>149</v>
       </c>
       <c r="B53" s="8">
         <v>53</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="20">
         <v>10100216</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="20" t="s">
         <v>216</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -16817,19 +16860,19 @@
       <c r="F53" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="G53" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="H53" s="5">
+      <c r="H53" s="20">
         <v>10100216</v>
       </c>
       <c r="I53" s="5">
         <v>10100216</v>
       </c>
-      <c r="J53" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K53" s="5" t="s">
+      <c r="J53" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K53" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L53" s="9">
@@ -16841,115 +16884,115 @@
       <c r="N53" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O53" s="1" t="s">
+      <c r="O53" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P53" s="9">
+      <c r="P53" s="22">
         <v>44916</v>
       </c>
-      <c r="Q53" s="5" t="s">
+      <c r="Q53" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R53" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S53" s="5" t="s">
+      <c r="R53" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S53" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T53" s="5" t="s">
+      <c r="T53" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U53" s="5" t="s">
+      <c r="U53" s="20" t="s">
         <v>1224</v>
       </c>
-      <c r="V53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W53" s="9">
+      <c r="V53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W53" s="22">
         <v>44882</v>
       </c>
-      <c r="X53" s="5" t="s">
+      <c r="X53" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Y53" s="1" t="s">
+      <c r="Y53" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="Z53" s="1" t="s">
+      <c r="Z53" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AA53" s="5" t="s">
+      <c r="AA53" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB53" s="5" t="s">
+      <c r="AB53" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AC53" s="5" t="s">
+      <c r="AC53" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD53" s="5" t="s">
+      <c r="AD53" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF53" s="5" t="s">
+      <c r="AE53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF53" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG53" s="5" t="s">
+      <c r="AG53" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH53" s="5" t="s">
+      <c r="AH53" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="AI53" s="5" t="s">
+      <c r="AI53" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ53" s="5" t="s">
+      <c r="AJ53" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL53" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM53" s="5" t="s">
+      <c r="AK53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL53" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM53" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN53" s="5" t="s">
+      <c r="AN53" s="20" t="s">
         <v>1690</v>
       </c>
-      <c r="AO53" s="5" t="s">
+      <c r="AO53" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP53" s="5" t="s">
+      <c r="AP53" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR53" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR53" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS53" s="5" t="s">
+      <c r="AQ53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR53" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR53" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS53" s="20" t="s">
         <v>2085</v>
       </c>
-      <c r="BT53" s="5" t="s">
+      <c r="BT53" s="20" t="s">
         <v>2081</v>
       </c>
-      <c r="BU53" s="5" t="s">
+      <c r="BU53" s="20" t="s">
         <v>2086</v>
       </c>
-      <c r="BV53" s="5" t="s">
+      <c r="BV53" s="20" t="s">
         <v>2086</v>
       </c>
-      <c r="BW53" s="5" t="s">
+      <c r="BW53" s="20" t="s">
         <v>2087</v>
       </c>
-      <c r="BX53" s="5" t="s">
+      <c r="BX53" s="20" t="s">
         <v>2088</v>
       </c>
     </row>
@@ -17975,17 +18018,17 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="61" spans="1:79" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:79" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>157</v>
       </c>
       <c r="B61" s="8">
         <v>61</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="20">
         <v>10100224</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="20" t="s">
         <v>240</v>
       </c>
       <c r="E61" s="5" t="s">
@@ -17994,19 +18037,19 @@
       <c r="F61" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="G61" s="5" t="s">
+      <c r="G61" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="H61" s="5">
+      <c r="H61" s="20">
         <v>10100224</v>
       </c>
       <c r="I61" s="5">
         <v>10100224</v>
       </c>
-      <c r="J61" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K61" s="5" t="s">
+      <c r="J61" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K61" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L61" s="9">
@@ -18018,124 +18061,124 @@
       <c r="N61" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O61" s="1" t="s">
+      <c r="O61" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P61" s="9">
+      <c r="P61" s="22">
         <v>44916</v>
       </c>
-      <c r="Q61" s="5" t="s">
+      <c r="Q61" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R61" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S61" s="5" t="s">
+      <c r="R61" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S61" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T61" s="5" t="s">
+      <c r="T61" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U61" s="5" t="s">
+      <c r="U61" s="20" t="s">
         <v>1232</v>
       </c>
-      <c r="V61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W61" s="9">
+      <c r="V61" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W61" s="22">
         <v>44882</v>
       </c>
-      <c r="X61" s="5" t="s">
+      <c r="X61" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Y61" s="1" t="s">
+      <c r="Y61" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="Z61" s="1" t="s">
+      <c r="Z61" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AA61" s="5" t="s">
+      <c r="AA61" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB61" s="5" t="s">
+      <c r="AB61" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AC61" s="5" t="s">
+      <c r="AC61" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD61" s="5" t="s">
+      <c r="AD61" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF61" s="5" t="s">
+      <c r="AE61" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF61" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG61" s="5" t="s">
+      <c r="AG61" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH61" s="5" t="s">
+      <c r="AH61" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AI61" s="5" t="s">
+      <c r="AI61" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ61" s="5" t="s">
+      <c r="AJ61" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL61" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM61" s="5" t="s">
+      <c r="AK61" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL61" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM61" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN61" s="5" t="s">
+      <c r="AN61" s="20" t="s">
         <v>1698</v>
       </c>
-      <c r="AO61" s="5" t="s">
+      <c r="AO61" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP61" s="5" t="s">
+      <c r="AP61" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR61" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR61" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS61" s="5" t="s">
+      <c r="AQ61" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR61" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR61" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS61" s="20" t="s">
         <v>2101</v>
       </c>
-      <c r="BT61" s="5" t="s">
+      <c r="BT61" s="20" t="s">
         <v>2102</v>
       </c>
-      <c r="BU61" s="5" t="s">
+      <c r="BU61" s="20" t="s">
         <v>2103</v>
       </c>
-      <c r="BV61" s="5" t="s">
+      <c r="BV61" s="20" t="s">
         <v>2107</v>
       </c>
-      <c r="BW61" s="5" t="s">
+      <c r="BW61" s="20" t="s">
         <v>2105</v>
       </c>
-      <c r="BX61" s="5" t="s">
+      <c r="BX61" s="20" t="s">
         <v>2106</v>
       </c>
-      <c r="BY61" s="5" t="s">
+      <c r="BY61" s="20" t="s">
         <v>2107</v>
       </c>
-      <c r="BZ61" s="5" t="s">
+      <c r="BZ61" s="20" t="s">
         <v>2107</v>
       </c>
-      <c r="CA61" s="5" t="s">
+      <c r="CA61" s="20" t="s">
         <v>2108</v>
       </c>
     </row>
@@ -25409,17 +25452,17 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="114" spans="1:76" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:76" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>84</v>
       </c>
       <c r="B114" s="8">
         <v>114</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C114" s="20">
         <v>10100112</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="20" t="s">
         <v>411</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -25428,19 +25471,19 @@
       <c r="F114" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="G114" s="5" t="s">
+      <c r="G114" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="H114" s="5">
+      <c r="H114" s="20">
         <v>10100112</v>
       </c>
       <c r="I114" s="5">
         <v>10100112</v>
       </c>
-      <c r="J114" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K114" s="5" t="s">
+      <c r="J114" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K114" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L114" s="9">
@@ -25452,115 +25495,115 @@
       <c r="N114" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O114" s="1" t="s">
+      <c r="O114" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P114" s="9">
+      <c r="P114" s="22">
         <v>44916</v>
       </c>
-      <c r="Q114" s="5" t="s">
+      <c r="Q114" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R114" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S114" s="5" t="s">
+      <c r="R114" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S114" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T114" s="5" t="s">
+      <c r="T114" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U114" s="5" t="s">
+      <c r="U114" s="20" t="s">
         <v>1284</v>
       </c>
-      <c r="V114" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W114" s="9">
+      <c r="V114" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W114" s="22">
         <v>44888</v>
       </c>
-      <c r="X114" s="5" t="s">
+      <c r="X114" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="Y114" s="1" t="s">
+      <c r="Y114" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="Z114" s="1" t="s">
+      <c r="Z114" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="AA114" s="5" t="s">
+      <c r="AA114" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB114" s="5" t="s">
+      <c r="AB114" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="AC114" s="5" t="s">
+      <c r="AC114" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD114" s="5" t="s">
+      <c r="AD114" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE114" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF114" s="5" t="s">
+      <c r="AE114" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF114" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG114" s="5" t="s">
+      <c r="AG114" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH114" s="5" t="s">
+      <c r="AH114" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="AI114" s="5" t="s">
+      <c r="AI114" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ114" s="5" t="s">
+      <c r="AJ114" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK114" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL114" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM114" s="5" t="s">
+      <c r="AK114" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL114" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM114" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN114" s="5" t="s">
+      <c r="AN114" s="20" t="s">
         <v>1741</v>
       </c>
-      <c r="AO114" s="5" t="s">
+      <c r="AO114" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP114" s="5" t="s">
+      <c r="AP114" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ114" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR114" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR114" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS114" s="5" t="s">
+      <c r="AQ114" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR114" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR114" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS114" s="20" t="s">
         <v>2173</v>
       </c>
-      <c r="BT114" s="5" t="s">
+      <c r="BT114" s="20" t="s">
         <v>2168</v>
       </c>
-      <c r="BU114" s="5" t="s">
+      <c r="BU114" s="20" t="s">
         <v>2169</v>
       </c>
-      <c r="BV114" s="5" t="s">
+      <c r="BV114" s="20" t="s">
         <v>2170</v>
       </c>
-      <c r="BW114" s="5" t="s">
+      <c r="BW114" s="20" t="s">
         <v>2171</v>
       </c>
-      <c r="BX114" s="5" t="s">
+      <c r="BX114" s="20" t="s">
         <v>2172</v>
       </c>
     </row>
@@ -29294,17 +29337,17 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="141" spans="1:80" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:80" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A141" s="5">
         <v>70</v>
       </c>
       <c r="B141" s="8">
         <v>141</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C141" s="20">
         <v>10100094</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="20" t="s">
         <v>495</v>
       </c>
       <c r="E141" s="5" t="s">
@@ -29313,19 +29356,19 @@
       <c r="F141" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="G141" s="5" t="s">
+      <c r="G141" s="20" t="s">
         <v>497</v>
       </c>
-      <c r="H141" s="5">
+      <c r="H141" s="20">
         <v>10100094</v>
       </c>
       <c r="I141" s="5">
         <v>10100094</v>
       </c>
-      <c r="J141" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K141" s="5" t="s">
+      <c r="J141" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K141" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L141" s="9">
@@ -29337,127 +29380,127 @@
       <c r="N141" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O141" s="1" t="s">
+      <c r="O141" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P141" s="9">
+      <c r="P141" s="22">
         <v>44916</v>
       </c>
-      <c r="Q141" s="5" t="s">
+      <c r="Q141" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R141" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S141" s="5" t="s">
+      <c r="R141" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S141" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T141" s="5" t="s">
+      <c r="T141" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U141" s="5" t="s">
+      <c r="U141" s="20" t="s">
         <v>1311</v>
       </c>
-      <c r="V141" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W141" s="9">
+      <c r="V141" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W141" s="22">
         <v>44888</v>
       </c>
-      <c r="X141" s="5" t="s">
+      <c r="X141" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="Y141" s="1" t="s">
+      <c r="Y141" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="Z141" s="1" t="s">
+      <c r="Z141" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="AA141" s="5" t="s">
+      <c r="AA141" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB141" s="5" t="s">
+      <c r="AB141" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="AC141" s="5" t="s">
+      <c r="AC141" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD141" s="5" t="s">
+      <c r="AD141" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE141" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF141" s="5" t="s">
+      <c r="AE141" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF141" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG141" s="5" t="s">
+      <c r="AG141" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH141" s="5" t="s">
+      <c r="AH141" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="AI141" s="5" t="s">
+      <c r="AI141" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ141" s="5" t="s">
+      <c r="AJ141" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK141" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL141" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM141" s="5" t="s">
+      <c r="AK141" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL141" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM141" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN141" s="5" t="s">
+      <c r="AN141" s="20" t="s">
         <v>1768</v>
       </c>
-      <c r="AO141" s="5" t="s">
+      <c r="AO141" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP141" s="5" t="s">
+      <c r="AP141" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ141" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR141" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR141" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS141" s="5" t="s">
+      <c r="AQ141" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR141" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR141" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS141" s="20" t="s">
         <v>2212</v>
       </c>
-      <c r="BT141" s="5" t="s">
+      <c r="BT141" s="20" t="s">
         <v>2213</v>
       </c>
-      <c r="BU141" s="5" t="s">
+      <c r="BU141" s="20" t="s">
         <v>2212</v>
       </c>
-      <c r="BV141" s="5" t="s">
+      <c r="BV141" s="20" t="s">
         <v>2213</v>
       </c>
-      <c r="BW141" s="5" t="s">
+      <c r="BW141" s="20" t="s">
         <v>2214</v>
       </c>
-      <c r="BX141" s="5" t="s">
+      <c r="BX141" s="20" t="s">
         <v>2215</v>
       </c>
-      <c r="BY141" s="5" t="s">
+      <c r="BY141" s="20" t="s">
         <v>2216</v>
       </c>
-      <c r="BZ141" s="5" t="s">
+      <c r="BZ141" s="20" t="s">
         <v>2217</v>
       </c>
-      <c r="CA141" s="5" t="s">
+      <c r="CA141" s="20" t="s">
         <v>2218</v>
       </c>
-      <c r="CB141" s="5" t="s">
+      <c r="CB141" s="20" t="s">
         <v>2219</v>
       </c>
     </row>
@@ -32175,17 +32218,17 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="161" spans="1:81" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:81" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A161" s="5">
         <v>57</v>
       </c>
       <c r="B161" s="8">
         <v>161</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C161" s="20">
         <v>10100079</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D161" s="20" t="s">
         <v>555</v>
       </c>
       <c r="E161" s="5" t="s">
@@ -32194,19 +32237,19 @@
       <c r="F161" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="G161" s="5" t="s">
+      <c r="G161" s="20" t="s">
         <v>557</v>
       </c>
-      <c r="H161" s="5">
+      <c r="H161" s="20">
         <v>10100079</v>
       </c>
       <c r="I161" s="5">
         <v>10100079</v>
       </c>
-      <c r="J161" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K161" s="5" t="s">
+      <c r="J161" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K161" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L161" s="9">
@@ -32218,130 +32261,130 @@
       <c r="N161" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O161" s="1" t="s">
+      <c r="O161" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P161" s="9">
+      <c r="P161" s="22">
         <v>44916</v>
       </c>
-      <c r="Q161" s="5" t="s">
+      <c r="Q161" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R161" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S161" s="5" t="s">
+      <c r="R161" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S161" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T161" s="5" t="s">
+      <c r="T161" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U161" s="5" t="s">
+      <c r="U161" s="20" t="s">
         <v>1331</v>
       </c>
-      <c r="V161" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W161" s="9">
+      <c r="V161" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W161" s="22">
         <v>44888</v>
       </c>
-      <c r="X161" s="5" t="s">
+      <c r="X161" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="Y161" s="1" t="s">
+      <c r="Y161" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="Z161" s="1" t="s">
+      <c r="Z161" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="AA161" s="5" t="s">
+      <c r="AA161" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB161" s="5" t="s">
+      <c r="AB161" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="AC161" s="5" t="s">
+      <c r="AC161" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD161" s="5" t="s">
+      <c r="AD161" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE161" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF161" s="5" t="s">
+      <c r="AE161" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF161" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG161" s="5" t="s">
+      <c r="AG161" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH161" s="5" t="s">
+      <c r="AH161" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="AI161" s="5" t="s">
+      <c r="AI161" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ161" s="5" t="s">
+      <c r="AJ161" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK161" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL161" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM161" s="5" t="s">
+      <c r="AK161" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL161" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM161" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN161" s="5" t="s">
+      <c r="AN161" s="20" t="s">
         <v>1788</v>
       </c>
-      <c r="AO161" s="5" t="s">
+      <c r="AO161" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP161" s="5" t="s">
+      <c r="AP161" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ161" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR161" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR161" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS161" s="5" t="s">
+      <c r="AQ161" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR161" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR161" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS161" s="20" t="s">
         <v>2243</v>
       </c>
-      <c r="BT161" s="5" t="s">
+      <c r="BT161" s="20" t="s">
         <v>2169</v>
       </c>
-      <c r="BU161" s="5" t="s">
+      <c r="BU161" s="20" t="s">
         <v>2244</v>
       </c>
-      <c r="BV161" s="5" t="s">
+      <c r="BV161" s="20" t="s">
         <v>2173</v>
       </c>
-      <c r="BW161" s="5" t="s">
+      <c r="BW161" s="20" t="s">
         <v>2170</v>
       </c>
-      <c r="BX161" s="5" t="s">
+      <c r="BX161" s="20" t="s">
         <v>2246</v>
       </c>
-      <c r="BY161" s="5" t="s">
+      <c r="BY161" s="20" t="s">
         <v>2245</v>
       </c>
-      <c r="BZ161" s="5" t="s">
+      <c r="BZ161" s="20" t="s">
         <v>2247</v>
       </c>
-      <c r="CA161" s="5" t="s">
+      <c r="CA161" s="20" t="s">
         <v>2247</v>
       </c>
-      <c r="CB161" s="5" t="s">
+      <c r="CB161" s="20" t="s">
         <v>2248</v>
       </c>
-      <c r="CC161" s="5" t="s">
+      <c r="CC161" s="20" t="s">
         <v>2232</v>
       </c>
     </row>
@@ -34249,17 +34292,17 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="175" spans="1:81" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:81" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A175" s="5">
         <v>13</v>
       </c>
       <c r="B175" s="8">
         <v>175</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C175" s="20">
         <v>10100014</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="20" t="s">
         <v>600</v>
       </c>
       <c r="E175" s="5" t="s">
@@ -34268,19 +34311,19 @@
       <c r="F175" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="G175" s="5" t="s">
+      <c r="G175" s="20" t="s">
         <v>602</v>
       </c>
-      <c r="H175" s="5">
+      <c r="H175" s="20">
         <v>10100014</v>
       </c>
       <c r="I175" s="5">
         <v>10100014</v>
       </c>
-      <c r="J175" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K175" s="5" t="s">
+      <c r="J175" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K175" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L175" s="9">
@@ -34292,115 +34335,115 @@
       <c r="N175" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O175" s="1" t="s">
+      <c r="O175" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P175" s="9">
+      <c r="P175" s="22">
         <v>44916</v>
       </c>
-      <c r="Q175" s="5" t="s">
+      <c r="Q175" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R175" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S175" s="5" t="s">
+      <c r="R175" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S175" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T175" s="5" t="s">
+      <c r="T175" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U175" s="5" t="s">
+      <c r="U175" s="20" t="s">
         <v>1343</v>
       </c>
-      <c r="V175" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W175" s="9">
+      <c r="V175" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W175" s="22">
         <v>44888</v>
       </c>
-      <c r="X175" s="5" t="s">
+      <c r="X175" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="Y175" s="1" t="s">
+      <c r="Y175" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="Z175" s="1" t="s">
+      <c r="Z175" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="AA175" s="5" t="s">
+      <c r="AA175" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB175" s="5" t="s">
+      <c r="AB175" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="AC175" s="5" t="s">
+      <c r="AC175" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD175" s="5" t="s">
+      <c r="AD175" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE175" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF175" s="5" t="s">
+      <c r="AE175" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF175" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG175" s="5" t="s">
+      <c r="AG175" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH175" s="5" t="s">
+      <c r="AH175" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="AI175" s="5" t="s">
+      <c r="AI175" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ175" s="5" t="s">
+      <c r="AJ175" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK175" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL175" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM175" s="5" t="s">
+      <c r="AK175" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL175" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM175" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN175" s="5" t="s">
+      <c r="AN175" s="20" t="s">
         <v>1801</v>
       </c>
-      <c r="AO175" s="5" t="s">
+      <c r="AO175" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP175" s="5" t="s">
+      <c r="AP175" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ175" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR175" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR175" s="5" t="s">
+      <c r="AQ175" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR175" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR175" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="BS175" s="5" t="s">
+      <c r="BS175" s="20" t="s">
         <v>2171</v>
       </c>
-      <c r="BT175" s="5" t="s">
+      <c r="BT175" s="20" t="s">
         <v>2171</v>
       </c>
-      <c r="BU175" s="5" t="s">
+      <c r="BU175" s="20" t="s">
         <v>2273</v>
       </c>
-      <c r="BV175" s="5" t="s">
+      <c r="BV175" s="20" t="s">
         <v>2274</v>
       </c>
-      <c r="BW175" s="5" t="s">
+      <c r="BW175" s="20" t="s">
         <v>2271</v>
       </c>
-      <c r="BX175" s="5" t="s">
+      <c r="BX175" s="20" t="s">
         <v>2275</v>
       </c>
     </row>
@@ -45378,17 +45421,17 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="250" spans="1:79" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:79" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A250" s="5">
         <v>201</v>
       </c>
       <c r="B250" s="8">
         <v>250</v>
       </c>
-      <c r="C250" s="5">
+      <c r="C250" s="20">
         <v>10100341</v>
       </c>
-      <c r="D250" s="5" t="s">
+      <c r="D250" s="20" t="s">
         <v>902</v>
       </c>
       <c r="E250" s="5" t="s">
@@ -45397,19 +45440,19 @@
       <c r="F250" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="G250" s="5" t="s">
+      <c r="G250" s="20" t="s">
         <v>904</v>
       </c>
-      <c r="H250" s="5">
+      <c r="H250" s="20">
         <v>10100341</v>
       </c>
       <c r="I250" s="5">
         <v>10100341</v>
       </c>
-      <c r="J250" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K250" s="5" t="s">
+      <c r="J250" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K250" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L250" s="9">
@@ -45421,124 +45464,124 @@
       <c r="N250" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O250" s="1" t="s">
+      <c r="O250" s="21" t="s">
         <v>1979</v>
       </c>
-      <c r="P250" s="9">
+      <c r="P250" s="22">
         <v>44916</v>
       </c>
-      <c r="Q250" s="5" t="s">
+      <c r="Q250" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R250" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S250" s="5" t="s">
+      <c r="R250" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S250" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T250" s="5" t="s">
+      <c r="T250" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U250" s="5" t="s">
+      <c r="U250" s="20" t="s">
         <v>1411</v>
       </c>
-      <c r="V250" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W250" s="9">
+      <c r="V250" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W250" s="22">
         <v>44888</v>
       </c>
-      <c r="X250" s="5" t="s">
+      <c r="X250" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="Y250" s="1" t="s">
+      <c r="Y250" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="Z250" s="1" t="s">
+      <c r="Z250" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="AA250" s="5" t="s">
+      <c r="AA250" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AB250" s="5" t="s">
+      <c r="AB250" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="AC250" s="5" t="s">
+      <c r="AC250" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="AD250" s="5" t="s">
+      <c r="AD250" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="AE250" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF250" s="5" t="s">
+      <c r="AE250" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF250" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="AG250" s="5" t="s">
+      <c r="AG250" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AH250" s="5" t="s">
+      <c r="AH250" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="AI250" s="5" t="s">
+      <c r="AI250" s="20" t="s">
         <v>1598</v>
       </c>
-      <c r="AJ250" s="5" t="s">
+      <c r="AJ250" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="AK250" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL250" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="AM250" s="5" t="s">
+      <c r="AK250" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL250" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="AM250" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AN250" s="5" t="s">
+      <c r="AN250" s="20" t="s">
         <v>1840</v>
       </c>
-      <c r="AO250" s="5" t="s">
+      <c r="AO250" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AP250" s="5" t="s">
+      <c r="AP250" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AQ250" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR250" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="BR250" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="BS250" s="5" t="s">
+      <c r="AQ250" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR250" s="20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="BR250" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="BS250" s="20" t="s">
         <v>2305</v>
       </c>
-      <c r="BT250" s="5" t="s">
+      <c r="BT250" s="20" t="s">
         <v>2306</v>
       </c>
-      <c r="BU250" s="5" t="s">
+      <c r="BU250" s="20" t="s">
         <v>2307</v>
       </c>
-      <c r="BV250" s="5" t="s">
+      <c r="BV250" s="20" t="s">
         <v>2069</v>
       </c>
-      <c r="BW250" s="5" t="s">
+      <c r="BW250" s="20" t="s">
         <v>2069</v>
       </c>
-      <c r="BX250" s="5" t="s">
+      <c r="BX250" s="20" t="s">
         <v>2069</v>
       </c>
-      <c r="BY250" s="5" t="s">
+      <c r="BY250" s="20" t="s">
         <v>2069</v>
       </c>
-      <c r="BZ250" s="5" t="s">
+      <c r="BZ250" s="20" t="s">
         <v>2069</v>
       </c>
-      <c r="CA250" s="5" t="s">
+      <c r="CA250" s="20" t="s">
         <v>2069</v>
       </c>
     </row>
@@ -48346,17 +48389,17 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="271" spans="1:86" ht="15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:86" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A271" s="5">
         <v>198</v>
       </c>
       <c r="B271" s="8">
         <v>271</v>
       </c>
-      <c r="C271" s="5">
+      <c r="C271" s="20">
         <v>10100308</v>
       </c>
-      <c r="D271" s="5" t="s">
+      <c r="D271" s="20" t="s">
         <v>970</v>
       </c>
       <c r="E271" s="5" t="s">
@@ -48365,19 +48408,19 @@
       <c r="F271" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="G271" s="5" t="s">
+      <c r="G271" s="20" t="s">
         <v>972</v>
       </c>
-      <c r="H271" s="5">
+      <c r="H271" s="20">
         <v>10100308</v>
       </c>
       <c r="I271" s="5">
         <v>10100308</v>
       </c>
-      <c r="J271" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K271" s="5" t="s">
+      <c r="J271" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K271" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L271" s="9">
@@ -48389,138 +48432,138 @@
       <c r="N271" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O271" s="1" t="s">
+      <c r="O271" s="21" t="s">
         <v>1952</v>
       </c>
-      <c r="P271" s="9">
+      <c r="P271" s="22">
         <v>44916</v>
       </c>
-      <c r="Q271" s="5" t="s">
+      <c r="Q271" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R271" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S271" s="5" t="s">
+      <c r="R271" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S271" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T271" s="5" t="s">
+      <c r="T271" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U271" s="5" t="s">
+      <c r="U271" s="20" t="s">
         <v>1432</v>
       </c>
-      <c r="V271" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W271" s="9">
+      <c r="V271" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W271" s="22">
         <v>44880</v>
       </c>
-      <c r="X271" s="5" t="s">
+      <c r="X271" s="20" t="s">
         <v>973</v>
       </c>
-      <c r="Y271" s="1" t="s">
+      <c r="Y271" s="21" t="s">
         <v>1975</v>
       </c>
-      <c r="Z271" s="1" t="s">
+      <c r="Z271" s="21" t="s">
         <v>974</v>
       </c>
-      <c r="AA271" s="5" t="s">
+      <c r="AA271" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AB271" s="5" t="s">
+      <c r="AB271" s="20" t="s">
         <v>975</v>
       </c>
-      <c r="AC271" s="5" t="s">
+      <c r="AC271" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AD271" s="5" t="s">
+      <c r="AD271" s="20" t="s">
         <v>976</v>
       </c>
-      <c r="AE271" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF271" s="5" t="s">
+      <c r="AE271" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF271" s="20" t="s">
         <v>1551</v>
       </c>
-      <c r="AG271" s="5" t="s">
+      <c r="AG271" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AH271" s="5" t="s">
+      <c r="AH271" s="20" t="s">
         <v>1990</v>
       </c>
-      <c r="AI271" s="5" t="s">
+      <c r="AI271" s="20" t="s">
         <v>977</v>
       </c>
-      <c r="AJ271" s="5" t="s">
+      <c r="AJ271" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AK271" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL271" s="5" t="s">
+      <c r="AK271" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL271" s="20" t="s">
         <v>1555</v>
       </c>
-      <c r="BS271" s="5" t="s">
+      <c r="BS271" s="20" t="s">
         <v>2000</v>
       </c>
-      <c r="BT271" s="5" t="s">
+      <c r="BT271" s="20" t="s">
         <v>2001</v>
       </c>
-      <c r="BU271" s="5" t="s">
+      <c r="BU271" s="20" t="s">
         <v>2002</v>
       </c>
-      <c r="BV271" s="5" t="s">
+      <c r="BV271" s="20" t="s">
         <v>2003</v>
       </c>
-      <c r="BW271" s="5" t="s">
+      <c r="BW271" s="20" t="s">
         <v>2002</v>
       </c>
-      <c r="BX271" s="5" t="s">
+      <c r="BX271" s="20" t="s">
         <v>2003</v>
       </c>
-      <c r="BY271" s="5" t="s">
+      <c r="BY271" s="20" t="s">
         <v>2002</v>
       </c>
-      <c r="BZ271" s="5" t="s">
+      <c r="BZ271" s="20" t="s">
         <v>2003</v>
       </c>
-      <c r="CA271" s="5" t="s">
+      <c r="CA271" s="20" t="s">
         <v>2004</v>
       </c>
-      <c r="CB271" s="5" t="s">
+      <c r="CB271" s="20" t="s">
         <v>2005</v>
       </c>
-      <c r="CC271" s="5" t="s">
+      <c r="CC271" s="20" t="s">
         <v>2004</v>
       </c>
-      <c r="CD271" s="5" t="s">
+      <c r="CD271" s="20" t="s">
         <v>2005</v>
       </c>
-      <c r="CE271" s="5" t="s">
+      <c r="CE271" s="20" t="s">
         <v>2006</v>
       </c>
-      <c r="CF271" s="5" t="s">
+      <c r="CF271" s="20" t="s">
         <v>2007</v>
       </c>
-      <c r="CG271" s="5" t="s">
+      <c r="CG271" s="20" t="s">
         <v>2006</v>
       </c>
-      <c r="CH271" s="5" t="s">
+      <c r="CH271" s="20" t="s">
         <v>2007</v>
       </c>
     </row>
-    <row r="272" spans="1:86" ht="15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:86" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A272" s="5">
         <v>199</v>
       </c>
       <c r="B272" s="8">
         <v>272</v>
       </c>
-      <c r="C272" s="5">
+      <c r="C272" s="20">
         <v>10100309</v>
       </c>
-      <c r="D272" s="5" t="s">
+      <c r="D272" s="20" t="s">
         <v>979</v>
       </c>
       <c r="E272" s="5" t="s">
@@ -48529,19 +48572,19 @@
       <c r="F272" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="G272" s="5" t="s">
+      <c r="G272" s="20" t="s">
         <v>981</v>
       </c>
-      <c r="H272" s="5">
+      <c r="H272" s="20">
         <v>10100309</v>
       </c>
       <c r="I272" s="5">
         <v>10100309</v>
       </c>
-      <c r="J272" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="K272" s="5" t="s">
+      <c r="J272" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K272" s="20" t="s">
         <v>1483</v>
       </c>
       <c r="L272" s="9">
@@ -48553,106 +48596,106 @@
       <c r="N272" s="10" t="s">
         <v>1536</v>
       </c>
-      <c r="O272" s="1" t="s">
+      <c r="O272" s="21" t="s">
         <v>1952</v>
       </c>
-      <c r="P272" s="9">
+      <c r="P272" s="22">
         <v>44916</v>
       </c>
-      <c r="Q272" s="5" t="s">
+      <c r="Q272" s="20" t="s">
         <v>1539</v>
       </c>
-      <c r="R272" s="5" t="s">
-        <v>1483</v>
-      </c>
-      <c r="S272" s="5" t="s">
+      <c r="R272" s="20" t="s">
+        <v>1483</v>
+      </c>
+      <c r="S272" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T272" s="5" t="s">
+      <c r="T272" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U272" s="5" t="s">
+      <c r="U272" s="20" t="s">
         <v>1433</v>
       </c>
-      <c r="V272" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W272" s="9">
+      <c r="V272" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W272" s="22">
         <v>44880</v>
       </c>
-      <c r="X272" s="5" t="s">
+      <c r="X272" s="20" t="s">
         <v>973</v>
       </c>
-      <c r="Y272" s="1" t="s">
+      <c r="Y272" s="21" t="s">
         <v>1975</v>
       </c>
-      <c r="Z272" s="1" t="s">
+      <c r="Z272" s="21" t="s">
         <v>974</v>
       </c>
-      <c r="AA272" s="5" t="s">
+      <c r="AA272" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AB272" s="5" t="s">
+      <c r="AB272" s="20" t="s">
         <v>975</v>
       </c>
-      <c r="AC272" s="5" t="s">
+      <c r="AC272" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AD272" s="5" t="s">
+      <c r="AD272" s="20" t="s">
         <v>976</v>
       </c>
-      <c r="AE272" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF272" s="5" t="s">
+      <c r="AE272" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF272" s="20" t="s">
         <v>1551</v>
       </c>
-      <c r="AG272" s="5" t="s">
+      <c r="AG272" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AH272" s="5" t="s">
+      <c r="AH272" s="20" t="s">
         <v>2008</v>
       </c>
-      <c r="AI272" s="5" t="s">
+      <c r="AI272" s="20" t="s">
         <v>977</v>
       </c>
-      <c r="AJ272" s="5" t="s">
+      <c r="AJ272" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AK272" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL272" s="5" t="s">
+      <c r="AK272" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL272" s="20" t="s">
         <v>1555</v>
       </c>
-      <c r="BS272" s="5" t="s">
+      <c r="BS272" s="20" t="s">
         <v>2009</v>
       </c>
-      <c r="BT272" s="5" t="s">
+      <c r="BT272" s="20" t="s">
         <v>2009</v>
       </c>
-      <c r="BU272" s="5" t="s">
+      <c r="BU272" s="20" t="s">
         <v>2009</v>
       </c>
-      <c r="BV272" s="5" t="s">
+      <c r="BV272" s="20" t="s">
         <v>2010</v>
       </c>
-      <c r="BW272" s="5" t="s">
+      <c r="BW272" s="20" t="s">
         <v>2010</v>
       </c>
-      <c r="BX272" s="5" t="s">
+      <c r="BX272" s="20" t="s">
         <v>2011</v>
       </c>
-      <c r="BY272" s="5" t="s">
+      <c r="BY272" s="20" t="s">
         <v>2012</v>
       </c>
-      <c r="BZ272" s="5" t="s">
+      <c r="BZ272" s="20" t="s">
         <v>2013</v>
       </c>
-      <c r="CA272" s="5" t="s">
+      <c r="CA272" s="20" t="s">
         <v>2014</v>
       </c>
-      <c r="CB272" s="5" t="s">
+      <c r="CB272" s="20" t="s">
         <v>2015</v>
       </c>
     </row>
@@ -56020,7 +56063,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BP324" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:CH324" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
IQC creator v1.0 20230103-001
</commit_message>
<xml_diff>
--- a/list_V02.xlsx
+++ b/list_V02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zz\PycharmProjects\IQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD682B-A286-4B25-B4CF-A532A9C69897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E68292-A570-4AB2-8B72-C998031B94F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" tabRatio="458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" tabRatio="458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9021,13 +9021,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:CH324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="AB323" sqref="AB4:AB323"/>
+      <selection pane="bottomLeft" activeCell="Y271" sqref="Y271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -49162,7 +49161,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="276" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A276" s="4">
         <v>373</v>
       </c>
@@ -49296,7 +49295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A277" s="4">
         <v>369</v>
       </c>
@@ -49448,7 +49447,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="278" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A278" s="4">
         <v>217</v>
       </c>
@@ -49588,7 +49587,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="279" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A279" s="4">
         <v>218</v>
       </c>
@@ -49740,7 +49739,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="280" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A280" s="4">
         <v>445</v>
       </c>
@@ -49883,7 +49882,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="281" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A281" s="4">
         <v>446</v>
       </c>
@@ -50032,7 +50031,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="282" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A282" s="4">
         <v>219</v>
       </c>
@@ -50172,7 +50171,7 @@
         <v>2319</v>
       </c>
     </row>
-    <row r="283" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A283" s="4">
         <v>222</v>
       </c>
@@ -50312,7 +50311,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="284" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A284" s="4">
         <v>216</v>
       </c>
@@ -50452,7 +50451,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="285" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A285" s="4">
         <v>221</v>
       </c>
@@ -50595,7 +50594,7 @@
         <v>2323</v>
       </c>
     </row>
-    <row r="286" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A286" s="4">
         <v>448</v>
       </c>
@@ -50735,7 +50734,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="287" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A287" s="4">
         <v>254</v>
       </c>
@@ -50887,7 +50886,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="288" spans="1:75" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:75" ht="15" x14ac:dyDescent="0.2">
       <c r="A288" s="4">
         <v>227</v>
       </c>
@@ -51033,7 +51032,7 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="289" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A289" s="4">
         <v>228</v>
       </c>
@@ -51179,7 +51178,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="290" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A290" s="4">
         <v>229</v>
       </c>
@@ -51319,7 +51318,7 @@
         <v>2333</v>
       </c>
     </row>
-    <row r="291" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A291" s="4">
         <v>231</v>
       </c>
@@ -51459,7 +51458,7 @@
         <v>2334</v>
       </c>
     </row>
-    <row r="292" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A292" s="4">
         <v>232</v>
       </c>
@@ -51599,7 +51598,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="293" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A293" s="4">
         <v>233</v>
       </c>
@@ -51739,7 +51738,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="294" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A294" s="4">
         <v>234</v>
       </c>
@@ -51879,7 +51878,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="295" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A295" s="4">
         <v>449</v>
       </c>
@@ -52019,7 +52018,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="296" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A296" s="4">
         <v>450</v>
       </c>
@@ -52159,7 +52158,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="297" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A297" s="4">
         <v>455</v>
       </c>
@@ -52299,7 +52298,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="298" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A298" s="4">
         <v>447</v>
       </c>
@@ -52439,7 +52438,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="299" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A299" s="4">
         <v>235</v>
       </c>
@@ -52579,7 +52578,7 @@
         <v>2336</v>
       </c>
     </row>
-    <row r="300" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A300" s="4">
         <v>456</v>
       </c>
@@ -52719,7 +52718,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="301" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A301" s="4">
         <v>376</v>
       </c>
@@ -52886,7 +52885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A302" s="4">
         <v>381</v>
       </c>
@@ -53056,7 +53055,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="303" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A303" s="4">
         <v>223</v>
       </c>
@@ -53178,7 +53177,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="304" spans="1:73" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:73" ht="15" x14ac:dyDescent="0.2">
       <c r="A304" s="4">
         <v>224</v>
       </c>
@@ -53318,7 +53317,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="305" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A305" s="4">
         <v>225</v>
       </c>
@@ -53461,7 +53460,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="306" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A306" s="4">
         <v>226</v>
       </c>
@@ -53601,7 +53600,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="307" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A307" s="4">
         <v>454</v>
       </c>
@@ -53719,7 +53718,7 @@
       <c r="BS307" s="10"/>
       <c r="BT307" s="10"/>
     </row>
-    <row r="308" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A308" s="4">
         <v>425</v>
       </c>
@@ -53859,7 +53858,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="309" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A309" s="4">
         <v>383</v>
       </c>
@@ -54029,7 +54028,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="310" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A310" s="4">
         <v>385</v>
       </c>
@@ -54181,7 +54180,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="311" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A311" s="4">
         <v>451</v>
       </c>
@@ -54297,7 +54296,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="312" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A312" s="4">
         <v>452</v>
       </c>
@@ -54413,7 +54412,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="313" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A313" s="4">
         <v>453</v>
       </c>
@@ -54529,7 +54528,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="314" spans="1:72" s="10" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:72" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A314" s="4">
         <v>466</v>
       </c>
@@ -54691,7 +54690,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="315" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A315" s="4">
         <v>238</v>
       </c>
@@ -54861,7 +54860,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="316" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A316" s="4">
         <v>245</v>
       </c>
@@ -55031,7 +55030,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="317" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A317" s="4">
         <v>255</v>
       </c>
@@ -55183,7 +55182,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="318" spans="1:72" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:72" ht="15" x14ac:dyDescent="0.2">
       <c r="A318" s="4">
         <v>253</v>
       </c>
@@ -55933,7 +55932,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="324" spans="1:70" s="10" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:70" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A324" s="4">
         <v>428</v>
       </c>
@@ -56096,14 +56095,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CH324" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="B"/>
-        <filter val="C"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:CH324" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>